<commit_message>
modifcata report-checklist con dettagli su gestione errori casi ID 29,37,45
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CIDITECHSRLXX/Ciditech/Point/6.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111CIDITECHSRLXX/Ciditech/Point/6.0/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fse\it-fse-accreditamento\GATEWAY\A1#111CIDITECHSRLXX\Ciditech\Point\V.6.0.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fse\it-fse-accreditamento\GATEWAY\A1#111CIDITECHSRLXX\Ciditech\Point\6.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB83C994-C1FE-4C4A-AD9C-9FE8EF9F0CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBDAF78-8357-47BA-9C20-C08D49C25489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25920" yWindow="2040" windowWidth="24000" windowHeight="12135" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="645" yWindow="1425" windowWidth="27750" windowHeight="13695" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -730,9 +730,6 @@
     <t>"Il servizio di validazione non risponde"</t>
   </si>
   <si>
-    <t>l'operazione deve essere ritentata successivamente</t>
-  </si>
-  <si>
     <t>campi non gestiti dall'applicazione</t>
   </si>
   <si>
@@ -778,9 +775,6 @@
     <t>Campo token JWT non valido: Il campo action_id non è corretto</t>
   </si>
   <si>
-    <t>il campo deve essere valorizzato correttamente; viene modificata di conseguenza la configurazione</t>
-  </si>
-  <si>
     <t>subject_application_id: Point</t>
   </si>
   <si>
@@ -788,6 +782,12 @@
   </si>
   <si>
     <t>subject_application_version: 6.0</t>
+  </si>
+  <si>
+    <t>il campo deve essere valorizzato correttamente; viene modificata di conseguenza la configurazione da parte del fornitore. Il medico può proseguire la creazione del documento, e procedere alla validazione in un secondo momento.</t>
+  </si>
+  <si>
+    <t>l'operazione deve essere ritentata successivamente; il documento rimane in stato"non validato"; un processo automatico si occupa di tentare l'invio ad intervalli regolari. L'elenco dei documenti "non validati" è visibile dagli utenti del sistema (medici), così da poter verificare lo stato e avvisare il fornitore in caso di anomalie persistenti</t>
   </si>
 </sst>
 </file>
@@ -3715,10 +3715,10 @@
   <dimension ref="A1:T627"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="J15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="B3" s="44"/>
       <c r="C3" s="49" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D3" s="40"/>
       <c r="F3" s="12"/>
@@ -3812,7 +3812,7 @@
       <c r="A4" s="45"/>
       <c r="B4" s="46"/>
       <c r="C4" s="49" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D4" s="40"/>
       <c r="E4" s="4"/>
@@ -3836,7 +3836,7 @@
       <c r="A5" s="47"/>
       <c r="B5" s="48"/>
       <c r="C5" s="49" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D5" s="40"/>
       <c r="F5" s="12"/>
@@ -3998,7 +3998,7 @@
         <v>110</v>
       </c>
       <c r="K10" s="34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L10" s="25"/>
       <c r="M10" s="25"/>
@@ -4036,7 +4036,7 @@
         <v>110</v>
       </c>
       <c r="K11" s="34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L11" s="25"/>
       <c r="M11" s="25"/>
@@ -4074,7 +4074,7 @@
         <v>110</v>
       </c>
       <c r="K12" s="34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L12" s="25"/>
       <c r="M12" s="25"/>
@@ -4112,7 +4112,7 @@
         <v>110</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L13" s="25"/>
       <c r="M13" s="25"/>
@@ -4149,10 +4149,10 @@
         <v>45189.352951388886</v>
       </c>
       <c r="H14" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="I14" s="24" t="s">
         <v>165</v>
-      </c>
-      <c r="I14" s="24" t="s">
-        <v>166</v>
       </c>
       <c r="J14" s="35" t="s">
         <v>54</v>
@@ -4165,13 +4165,13 @@
         <v>54</v>
       </c>
       <c r="N14" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O14" s="25" t="s">
         <v>54</v>
       </c>
       <c r="P14" s="25" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="Q14" s="35" t="s">
         <v>108</v>
@@ -4182,7 +4182,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="102.75" customHeight="1" thickBot="1">
+    <row r="15" spans="1:20" ht="153" customHeight="1" thickBot="1">
       <c r="A15" s="20">
         <v>37</v>
       </c>
@@ -4205,10 +4205,10 @@
         <v>45189.356828703705</v>
       </c>
       <c r="H15" s="33" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J15" s="35" t="s">
         <v>54</v>
@@ -4221,13 +4221,13 @@
         <v>54</v>
       </c>
       <c r="N15" s="35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O15" s="25" t="s">
         <v>54</v>
       </c>
       <c r="P15" s="25" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="Q15" s="35" t="s">
         <v>108</v>
@@ -4238,7 +4238,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="122.25" customHeight="1" thickBot="1">
+    <row r="16" spans="1:20" ht="197.25" customHeight="1" thickBot="1">
       <c r="A16" s="20">
         <v>45</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>110</v>
       </c>
       <c r="P16" s="25" t="s">
-        <v>154</v>
+        <v>173</v>
       </c>
       <c r="Q16" s="35" t="s">
         <v>108</v>
@@ -4312,7 +4312,7 @@
         <v>110</v>
       </c>
       <c r="K17" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L17" s="25"/>
       <c r="M17" s="25"/>
@@ -4350,7 +4350,7 @@
         <v>110</v>
       </c>
       <c r="K18" s="25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L18" s="25"/>
       <c r="M18" s="25"/>
@@ -4388,7 +4388,7 @@
         <v>110</v>
       </c>
       <c r="K19" s="25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L19" s="25"/>
       <c r="M19" s="25"/>
@@ -4426,7 +4426,7 @@
         <v>110</v>
       </c>
       <c r="K20" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L20" s="25"/>
       <c r="M20" s="25"/>
@@ -4464,7 +4464,7 @@
         <v>110</v>
       </c>
       <c r="K21" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L21" s="25"/>
       <c r="M21" s="25"/>
@@ -4502,7 +4502,7 @@
         <v>110</v>
       </c>
       <c r="K22" s="25" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L22" s="25"/>
       <c r="M22" s="25"/>
@@ -4540,7 +4540,7 @@
         <v>110</v>
       </c>
       <c r="K23" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L23" s="25"/>
       <c r="M23" s="25"/>
@@ -4578,7 +4578,7 @@
         <v>110</v>
       </c>
       <c r="K24" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L24" s="25"/>
       <c r="M24" s="25"/>
@@ -4616,7 +4616,7 @@
         <v>110</v>
       </c>
       <c r="K25" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L25" s="25"/>
       <c r="M25" s="25"/>
@@ -4654,7 +4654,7 @@
         <v>110</v>
       </c>
       <c r="K26" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L26" s="25"/>
       <c r="M26" s="25"/>
@@ -4692,7 +4692,7 @@
         <v>110</v>
       </c>
       <c r="K27" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L27" s="25"/>
       <c r="M27" s="25"/>
@@ -4730,7 +4730,7 @@
         <v>110</v>
       </c>
       <c r="K28" s="25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L28" s="25"/>
       <c r="M28" s="25"/>
@@ -9151,7 +9151,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>